<commit_message>
enhance plotting macros (behavior macros) add a trace view generally shrink the figure size adjust the beamplot
</commit_message>
<xml_diff>
--- a/cook/head_fixed_training_sensory_prediction/status_report.xlsx
+++ b/cook/head_fixed_training_sensory_prediction/status_report.xlsx
@@ -61,15 +61,18 @@
     <t>SensoryPrediction_202510</t>
   </si>
   <si>
+    <t>RSS4</t>
+  </si>
+  <si>
     <t>QYV5M</t>
   </si>
   <si>
-    <t>RSS4</t>
-  </si>
-  <si>
     <t>HFT</t>
   </si>
   <si>
+    <t>20251006</t>
+  </si>
+  <si>
     <t>20251007</t>
   </si>
   <si>
@@ -82,7 +85,7 @@
     <t>20251010</t>
   </si>
   <si>
-    <t>20251006</t>
+    <t>20251006_RSS4_1_day0</t>
   </si>
   <si>
     <t>20251007_QYV5M_1_day0</t>
@@ -91,6 +94,12 @@
     <t>20251007_QYV5M_2_day0</t>
   </si>
   <si>
+    <t>20251007_RSS4_2_day0</t>
+  </si>
+  <si>
+    <t>20251007_RSS4_3_day0</t>
+  </si>
+  <si>
     <t>20251008_QYV5M_cuedpuff_1_cuedpuff100</t>
   </si>
   <si>
@@ -106,6 +115,21 @@
     <t>20251008_QYV5M_cuedpuff_5_cuedpuff100</t>
   </si>
   <si>
+    <t>20251008_RSS4_cuedpuff_1_cuedpuff100</t>
+  </si>
+  <si>
+    <t>20251008_RSS4_cuedpuff_2_cuedpuff100</t>
+  </si>
+  <si>
+    <t>20251008_RSS4_cuedpuff_3_cuedpuff100</t>
+  </si>
+  <si>
+    <t>20251008_RSS4_cuedpuff_4_cuedpuff100</t>
+  </si>
+  <si>
+    <t>20251008_RSS4_cuedpuff_5_cuedpuff100</t>
+  </si>
+  <si>
     <t>20251009_QYV5M_cuedpuff_1_cuedpuff100</t>
   </si>
   <si>
@@ -121,6 +145,21 @@
     <t>20251009_QYV5M_cuedpuff_5_cuedpuff90</t>
   </si>
   <si>
+    <t>20251009_RSS4_cuedpuff_1_cuedpuff100</t>
+  </si>
+  <si>
+    <t>20251009_RSS4_cuedpuff_2_cuedpuff100</t>
+  </si>
+  <si>
+    <t>20251009_RSS4_cuedpuff_3_cuedpuff90</t>
+  </si>
+  <si>
+    <t>20251009_RSS4_cuedpuff_4_cuedpuff90</t>
+  </si>
+  <si>
+    <t>20251009_RSS4_cuedpuff_5_cuedpuff90</t>
+  </si>
+  <si>
     <t>20251010_QYV5M_cuedpuff_1_cuedpuff90</t>
   </si>
   <si>
@@ -134,45 +173,6 @@
   </si>
   <si>
     <t>20251010_QYV5M_cuedpuff_5_cuedpuff90</t>
-  </si>
-  <si>
-    <t>20251006_RSS4_1_day0</t>
-  </si>
-  <si>
-    <t>20251007_RSS4_2_day0</t>
-  </si>
-  <si>
-    <t>20251007_RSS4_3_day0</t>
-  </si>
-  <si>
-    <t>20251008_RSS4_cuedpuff_1_cuedpuff100</t>
-  </si>
-  <si>
-    <t>20251008_RSS4_cuedpuff_2_cuedpuff100</t>
-  </si>
-  <si>
-    <t>20251008_RSS4_cuedpuff_3_cuedpuff100</t>
-  </si>
-  <si>
-    <t>20251008_RSS4_cuedpuff_4_cuedpuff100</t>
-  </si>
-  <si>
-    <t>20251008_RSS4_cuedpuff_5_cuedpuff100</t>
-  </si>
-  <si>
-    <t>20251009_RSS4_cuedpuff_1_cuedpuff100</t>
-  </si>
-  <si>
-    <t>20251009_RSS4_cuedpuff_2_cuedpuff100</t>
-  </si>
-  <si>
-    <t>20251009_RSS4_cuedpuff_3_cuedpuff90</t>
-  </si>
-  <si>
-    <t>20251009_RSS4_cuedpuff_4_cuedpuff90</t>
-  </si>
-  <si>
-    <t>20251009_RSS4_cuedpuff_5_cuedpuff90</t>
   </si>
   <si>
     <t>20251010_RSS4_cuedpuff_1_cuedpuff90</t>
@@ -219,7 +219,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF1A4E86"/>
+      <color rgb="FFFF7F0E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,7 +243,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFF28E2B"/>
+      <color rgb="FF1F77B4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -690,14 +690,14 @@
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>24</v>
@@ -734,8 +734,8 @@
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
+      <c r="B4" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>17</v>
@@ -866,14 +866,14 @@
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
+      <c r="B7" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>28</v>
@@ -910,14 +910,14 @@
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>29</v>
@@ -954,8 +954,8 @@
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
+      <c r="B9" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
@@ -998,8 +998,8 @@
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
+      <c r="B10" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
@@ -1042,8 +1042,8 @@
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
+      <c r="B11" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
@@ -1181,7 +1181,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>35</v>
@@ -1225,7 +1225,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>36</v>
@@ -1269,7 +1269,7 @@
         <v>17</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>37</v>
@@ -1306,8 +1306,8 @@
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>15</v>
+      <c r="B17" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>17</v>
@@ -1350,8 +1350,8 @@
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>15</v>
+      <c r="B18" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>17</v>
@@ -1401,7 +1401,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>40</v>
@@ -1445,7 +1445,7 @@
         <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>41</v>
@@ -1489,7 +1489,7 @@
         <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>42</v>
@@ -1526,14 +1526,14 @@
       <c r="A22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>16</v>
+      <c r="B22" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>43</v>
@@ -1570,14 +1570,14 @@
       <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>16</v>
+      <c r="B23" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>44</v>
@@ -1614,14 +1614,14 @@
       <c r="A24" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>16</v>
+      <c r="B24" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>45</v>
@@ -1658,14 +1658,14 @@
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>16</v>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>46</v>
@@ -1702,14 +1702,14 @@
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>16</v>
+      <c r="B26" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>47</v>
@@ -1753,7 +1753,7 @@
         <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>48</v>
@@ -1797,7 +1797,7 @@
         <v>17</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>49</v>
@@ -1841,7 +1841,7 @@
         <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>50</v>
@@ -1885,7 +1885,7 @@
         <v>17</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>51</v>
@@ -1929,7 +1929,7 @@
         <v>17</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>52</v>
@@ -1966,14 +1966,14 @@
       <c r="A32" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>16</v>
+      <c r="B32" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>53</v>
@@ -2010,14 +2010,14 @@
       <c r="A33" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>16</v>
+      <c r="B33" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>54</v>
@@ -2054,14 +2054,14 @@
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>16</v>
+      <c r="B34" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>55</v>
@@ -2098,14 +2098,14 @@
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>16</v>
+      <c r="B35" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>56</v>
@@ -2142,14 +2142,14 @@
       <c r="A36" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>16</v>
+      <c r="B36" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>57</v>

</xml_diff>